<commit_message>
Add HCAO label search for CL & HsapDv IDs
</commit_message>
<xml_diff>
--- a/metadata/bcb61471-2a44-4d00-a0af-ff085512674c_0b75c598-0893-4216-afe8-5414cab7739d_dcp.xlsx
+++ b/metadata/bcb61471-2a44-4d00-a0af-ff085512674c_0b75c598-0893-4216-afe8-5414cab7739d_dcp.xlsx
@@ -4423,7 +4423,11 @@
           <t>60-69</t>
         </is>
       </c>
-      <c r="W6" t="inlineStr"/>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr"/>
@@ -4534,7 +4538,11 @@
           <t>60-69</t>
         </is>
       </c>
-      <c r="W7" t="inlineStr"/>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
@@ -4645,7 +4653,11 @@
           <t>50-59</t>
         </is>
       </c>
-      <c r="W8" t="inlineStr"/>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr"/>
@@ -4756,7 +4768,11 @@
           <t>50-59</t>
         </is>
       </c>
-      <c r="W9" t="inlineStr"/>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr"/>
@@ -4867,7 +4883,11 @@
           <t>60-69</t>
         </is>
       </c>
-      <c r="W10" t="inlineStr"/>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr"/>
@@ -4978,7 +4998,11 @@
           <t>50-59</t>
         </is>
       </c>
-      <c r="W11" t="inlineStr"/>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr"/>
@@ -5093,7 +5117,11 @@
           <t>50-59</t>
         </is>
       </c>
-      <c r="W12" t="inlineStr"/>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr"/>
@@ -17399,7 +17427,7 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>na||na</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
@@ -17421,7 +17449,7 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t>CL:0000235</t>
+          <t>CL:0000235||macrophage</t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>

</xml_diff>

<commit_message>
Shorten organism_ontology_term_id conversion with tissue_type_taxon function
</commit_message>
<xml_diff>
--- a/metadata/bcb61471-2a44-4d00-a0af-ff085512674c_0b75c598-0893-4216-afe8-5414cab7739d_dcp.xlsx
+++ b/metadata/bcb61471-2a44-4d00-a0af-ff085512674c_0b75c598-0893-4216-afe8-5414cab7739d_dcp.xlsx
@@ -12280,7 +12280,11 @@
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
@@ -12358,7 +12362,11 @@
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
@@ -12436,7 +12444,11 @@
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
@@ -12514,7 +12526,11 @@
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
@@ -12592,7 +12608,11 @@
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
@@ -12670,7 +12690,11 @@
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
@@ -12748,7 +12772,11 @@
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
@@ -12826,7 +12854,11 @@
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
@@ -12904,7 +12936,11 @@
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -12982,7 +13018,11 @@
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
@@ -13060,7 +13100,11 @@
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
@@ -13138,7 +13182,11 @@
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
@@ -13216,7 +13264,11 @@
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
@@ -13294,7 +13346,11 @@
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
@@ -13372,7 +13428,11 @@
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
@@ -13450,7 +13510,11 @@
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
@@ -13528,7 +13592,11 @@
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
@@ -13606,7 +13674,11 @@
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
@@ -13684,7 +13756,11 @@
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
@@ -13762,7 +13838,11 @@
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
@@ -13840,7 +13920,11 @@
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
@@ -13918,7 +14002,11 @@
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
@@ -13996,7 +14084,11 @@
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
@@ -14074,7 +14166,11 @@
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
@@ -14152,7 +14248,11 @@
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
@@ -14230,7 +14330,11 @@
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
@@ -14308,7 +14412,11 @@
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
@@ -14386,7 +14494,11 @@
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
@@ -14464,7 +14576,11 @@
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
@@ -14542,7 +14658,11 @@
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
@@ -14620,7 +14740,11 @@
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
@@ -14698,7 +14822,11 @@
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>9606</t>
+        </is>
+      </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
@@ -17427,7 +17555,7 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>na||na</t>
+          <t>na</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
@@ -17449,7 +17577,7 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t>CL:0000235||macrophage</t>
+          <t>macrophage</t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>

</xml_diff>

<commit_message>
Assign protocol_ids to entities
</commit_message>
<xml_diff>
--- a/metadata/bcb61471-2a44-4d00-a0af-ff085512674c_0b75c598-0893-4216-afe8-5414cab7739d_dcp.xlsx
+++ b/metadata/bcb61471-2a44-4d00-a0af-ff085512674c_0b75c598-0893-4216-afe8-5414cab7739d_dcp.xlsx
@@ -6742,7 +6742,11 @@
           <t>IpiNivo_Complete</t>
         </is>
       </c>
-      <c r="BA6" t="inlineStr"/>
+      <c r="BA6" t="inlineStr">
+        <is>
+          <t>collection_protocol_1</t>
+        </is>
+      </c>
       <c r="BB6" t="inlineStr"/>
       <c r="BC6" t="inlineStr"/>
       <c r="BD6" t="inlineStr"/>
@@ -6863,7 +6867,11 @@
           <t>IpiNivo_Complete</t>
         </is>
       </c>
-      <c r="BA7" t="inlineStr"/>
+      <c r="BA7" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB7" t="inlineStr"/>
       <c r="BC7" t="inlineStr"/>
       <c r="BD7" t="inlineStr"/>
@@ -6980,7 +6988,11 @@
           <t>IpiNivo_Complete</t>
         </is>
       </c>
-      <c r="BA8" t="inlineStr"/>
+      <c r="BA8" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB8" t="inlineStr"/>
       <c r="BC8" t="inlineStr"/>
       <c r="BD8" t="inlineStr"/>
@@ -7097,7 +7109,11 @@
           <t>IpiNivo_Complete</t>
         </is>
       </c>
-      <c r="BA9" t="inlineStr"/>
+      <c r="BA9" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB9" t="inlineStr"/>
       <c r="BC9" t="inlineStr"/>
       <c r="BD9" t="inlineStr"/>
@@ -7214,7 +7230,11 @@
           <t>IpiNivo_Complete</t>
         </is>
       </c>
-      <c r="BA10" t="inlineStr"/>
+      <c r="BA10" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB10" t="inlineStr"/>
       <c r="BC10" t="inlineStr"/>
       <c r="BD10" t="inlineStr"/>
@@ -7331,7 +7351,11 @@
           <t>IpiNivo_Mixed</t>
         </is>
       </c>
-      <c r="BA11" t="inlineStr"/>
+      <c r="BA11" t="inlineStr">
+        <is>
+          <t>collection_protocol_1</t>
+        </is>
+      </c>
       <c r="BB11" t="inlineStr"/>
       <c r="BC11" t="inlineStr"/>
       <c r="BD11" t="inlineStr"/>
@@ -7448,7 +7472,11 @@
           <t>IpiNivo_Mixed</t>
         </is>
       </c>
-      <c r="BA12" t="inlineStr"/>
+      <c r="BA12" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB12" t="inlineStr"/>
       <c r="BC12" t="inlineStr"/>
       <c r="BD12" t="inlineStr"/>
@@ -7561,7 +7589,11 @@
           <t>IpiNivo_Mixed</t>
         </is>
       </c>
-      <c r="BA13" t="inlineStr"/>
+      <c r="BA13" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB13" t="inlineStr"/>
       <c r="BC13" t="inlineStr"/>
       <c r="BD13" t="inlineStr"/>
@@ -7674,7 +7706,11 @@
           <t>IpiNivo_Mixed</t>
         </is>
       </c>
-      <c r="BA14" t="inlineStr"/>
+      <c r="BA14" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB14" t="inlineStr"/>
       <c r="BC14" t="inlineStr"/>
       <c r="BD14" t="inlineStr"/>
@@ -7787,7 +7823,11 @@
           <t>IpiNivo_Mixed</t>
         </is>
       </c>
-      <c r="BA15" t="inlineStr"/>
+      <c r="BA15" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB15" t="inlineStr"/>
       <c r="BC15" t="inlineStr"/>
       <c r="BD15" t="inlineStr"/>
@@ -7904,7 +7944,11 @@
           <t>IpiNivo_Resistant</t>
         </is>
       </c>
-      <c r="BA16" t="inlineStr"/>
+      <c r="BA16" t="inlineStr">
+        <is>
+          <t>collection_protocol_1</t>
+        </is>
+      </c>
       <c r="BB16" t="inlineStr"/>
       <c r="BC16" t="inlineStr"/>
       <c r="BD16" t="inlineStr"/>
@@ -8021,7 +8065,11 @@
           <t>IpiNivo_Resistant</t>
         </is>
       </c>
-      <c r="BA17" t="inlineStr"/>
+      <c r="BA17" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB17" t="inlineStr"/>
       <c r="BC17" t="inlineStr"/>
       <c r="BD17" t="inlineStr"/>
@@ -8134,7 +8182,11 @@
           <t>IpiNivo_Resistant</t>
         </is>
       </c>
-      <c r="BA18" t="inlineStr"/>
+      <c r="BA18" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB18" t="inlineStr"/>
       <c r="BC18" t="inlineStr"/>
       <c r="BD18" t="inlineStr"/>
@@ -8247,7 +8299,11 @@
           <t>IpiNivo_Resistant</t>
         </is>
       </c>
-      <c r="BA19" t="inlineStr"/>
+      <c r="BA19" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB19" t="inlineStr"/>
       <c r="BC19" t="inlineStr"/>
       <c r="BD19" t="inlineStr"/>
@@ -8360,7 +8416,11 @@
           <t>IpiNivo_Resistant</t>
         </is>
       </c>
-      <c r="BA20" t="inlineStr"/>
+      <c r="BA20" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB20" t="inlineStr"/>
       <c r="BC20" t="inlineStr"/>
       <c r="BD20" t="inlineStr"/>
@@ -8473,7 +8533,11 @@
           <t>IpiNivo_Resistant</t>
         </is>
       </c>
-      <c r="BA21" t="inlineStr"/>
+      <c r="BA21" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB21" t="inlineStr"/>
       <c r="BC21" t="inlineStr"/>
       <c r="BD21" t="inlineStr"/>
@@ -8574,7 +8638,11 @@
           <t>NivoExposed</t>
         </is>
       </c>
-      <c r="BA22" t="inlineStr"/>
+      <c r="BA22" t="inlineStr">
+        <is>
+          <t>collection_protocol_1</t>
+        </is>
+      </c>
       <c r="BB22" t="inlineStr"/>
       <c r="BC22" t="inlineStr"/>
       <c r="BD22" t="inlineStr"/>
@@ -8675,7 +8743,11 @@
           <t>NivoExposed</t>
         </is>
       </c>
-      <c r="BA23" t="inlineStr"/>
+      <c r="BA23" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB23" t="inlineStr"/>
       <c r="BC23" t="inlineStr"/>
       <c r="BD23" t="inlineStr"/>
@@ -8776,7 +8848,11 @@
           <t>NivoExposed</t>
         </is>
       </c>
-      <c r="BA24" t="inlineStr"/>
+      <c r="BA24" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB24" t="inlineStr"/>
       <c r="BC24" t="inlineStr"/>
       <c r="BD24" t="inlineStr"/>
@@ -8877,7 +8953,11 @@
           <t>NivoExposed</t>
         </is>
       </c>
-      <c r="BA25" t="inlineStr"/>
+      <c r="BA25" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB25" t="inlineStr"/>
       <c r="BC25" t="inlineStr"/>
       <c r="BD25" t="inlineStr"/>
@@ -8978,7 +9058,11 @@
           <t>NivoExposed</t>
         </is>
       </c>
-      <c r="BA26" t="inlineStr"/>
+      <c r="BA26" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB26" t="inlineStr"/>
       <c r="BC26" t="inlineStr"/>
       <c r="BD26" t="inlineStr"/>
@@ -9095,7 +9179,11 @@
           <t>UT1</t>
         </is>
       </c>
-      <c r="BA27" t="inlineStr"/>
+      <c r="BA27" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB27" t="inlineStr"/>
       <c r="BC27" t="inlineStr"/>
       <c r="BD27" t="inlineStr"/>
@@ -9208,7 +9296,11 @@
           <t>UT1</t>
         </is>
       </c>
-      <c r="BA28" t="inlineStr"/>
+      <c r="BA28" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB28" t="inlineStr"/>
       <c r="BC28" t="inlineStr"/>
       <c r="BD28" t="inlineStr"/>
@@ -9321,7 +9413,11 @@
           <t>UT1</t>
         </is>
       </c>
-      <c r="BA29" t="inlineStr"/>
+      <c r="BA29" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB29" t="inlineStr"/>
       <c r="BC29" t="inlineStr"/>
       <c r="BD29" t="inlineStr"/>
@@ -9434,7 +9530,11 @@
           <t>UT1</t>
         </is>
       </c>
-      <c r="BA30" t="inlineStr"/>
+      <c r="BA30" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB30" t="inlineStr"/>
       <c r="BC30" t="inlineStr"/>
       <c r="BD30" t="inlineStr"/>
@@ -9539,7 +9639,11 @@
           <t>UT2</t>
         </is>
       </c>
-      <c r="BA31" t="inlineStr"/>
+      <c r="BA31" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB31" t="inlineStr"/>
       <c r="BC31" t="inlineStr"/>
       <c r="BD31" t="inlineStr"/>
@@ -9640,7 +9744,11 @@
           <t>UT2</t>
         </is>
       </c>
-      <c r="BA32" t="inlineStr"/>
+      <c r="BA32" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB32" t="inlineStr"/>
       <c r="BC32" t="inlineStr"/>
       <c r="BD32" t="inlineStr"/>
@@ -9741,7 +9849,11 @@
           <t>UT2</t>
         </is>
       </c>
-      <c r="BA33" t="inlineStr"/>
+      <c r="BA33" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB33" t="inlineStr"/>
       <c r="BC33" t="inlineStr"/>
       <c r="BD33" t="inlineStr"/>
@@ -9842,7 +9954,11 @@
           <t>UT2</t>
         </is>
       </c>
-      <c r="BA34" t="inlineStr"/>
+      <c r="BA34" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB34" t="inlineStr"/>
       <c r="BC34" t="inlineStr"/>
       <c r="BD34" t="inlineStr"/>
@@ -9959,7 +10075,11 @@
           <t>IpiNivo_Complete</t>
         </is>
       </c>
-      <c r="BA35" t="inlineStr"/>
+      <c r="BA35" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB35" t="inlineStr"/>
       <c r="BC35" t="inlineStr"/>
       <c r="BD35" t="inlineStr"/>
@@ -10064,7 +10184,11 @@
           <t>IpiNivo_Mixed</t>
         </is>
       </c>
-      <c r="BA36" t="inlineStr"/>
+      <c r="BA36" t="inlineStr">
+        <is>
+          <t>collection_protocol_1</t>
+        </is>
+      </c>
       <c r="BB36" t="inlineStr"/>
       <c r="BC36" t="inlineStr"/>
       <c r="BD36" t="inlineStr"/>
@@ -10169,7 +10293,11 @@
           <t>IpiNivo_Mixed</t>
         </is>
       </c>
-      <c r="BA37" t="inlineStr"/>
+      <c r="BA37" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB37" t="inlineStr"/>
       <c r="BC37" t="inlineStr"/>
       <c r="BD37" t="inlineStr"/>
@@ -10270,7 +10398,11 @@
           <t>IpiNivo_Mixed</t>
         </is>
       </c>
-      <c r="BA38" t="inlineStr"/>
+      <c r="BA38" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB38" t="inlineStr"/>
       <c r="BC38" t="inlineStr"/>
       <c r="BD38" t="inlineStr"/>
@@ -10371,7 +10503,11 @@
           <t>IpiNivo_Mixed</t>
         </is>
       </c>
-      <c r="BA39" t="inlineStr"/>
+      <c r="BA39" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB39" t="inlineStr"/>
       <c r="BC39" t="inlineStr"/>
       <c r="BD39" t="inlineStr"/>
@@ -10472,7 +10608,11 @@
           <t>IpiNivo_Mixed</t>
         </is>
       </c>
-      <c r="BA40" t="inlineStr"/>
+      <c r="BA40" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB40" t="inlineStr"/>
       <c r="BC40" t="inlineStr"/>
       <c r="BD40" t="inlineStr"/>
@@ -10577,7 +10717,11 @@
           <t>NivoExposed</t>
         </is>
       </c>
-      <c r="BA41" t="inlineStr"/>
+      <c r="BA41" t="inlineStr">
+        <is>
+          <t>collection_protocol_1</t>
+        </is>
+      </c>
       <c r="BB41" t="inlineStr"/>
       <c r="BC41" t="inlineStr"/>
       <c r="BD41" t="inlineStr"/>
@@ -10682,7 +10826,11 @@
           <t>NivoExposed</t>
         </is>
       </c>
-      <c r="BA42" t="inlineStr"/>
+      <c r="BA42" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB42" t="inlineStr"/>
       <c r="BC42" t="inlineStr"/>
       <c r="BD42" t="inlineStr"/>
@@ -10783,7 +10931,11 @@
           <t>NivoExposed</t>
         </is>
       </c>
-      <c r="BA43" t="inlineStr"/>
+      <c r="BA43" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB43" t="inlineStr"/>
       <c r="BC43" t="inlineStr"/>
       <c r="BD43" t="inlineStr"/>
@@ -10884,7 +11036,11 @@
           <t>NivoExposed</t>
         </is>
       </c>
-      <c r="BA44" t="inlineStr"/>
+      <c r="BA44" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB44" t="inlineStr"/>
       <c r="BC44" t="inlineStr"/>
       <c r="BD44" t="inlineStr"/>
@@ -10985,7 +11141,11 @@
           <t>NivoExposed</t>
         </is>
       </c>
-      <c r="BA45" t="inlineStr"/>
+      <c r="BA45" t="inlineStr">
+        <is>
+          <t>collection_protocol_2</t>
+        </is>
+      </c>
       <c r="BB45" t="inlineStr"/>
       <c r="BC45" t="inlineStr"/>
       <c r="BD45" t="inlineStr"/>
@@ -12987,7 +13147,11 @@
         </is>
       </c>
       <c r="AP14" t="inlineStr"/>
-      <c r="AQ14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr">
+        <is>
+          <t>enrichment_protocol_1</t>
+        </is>
+      </c>
       <c r="AR14" t="inlineStr"/>
       <c r="AS14" t="inlineStr"/>
       <c r="AT14" t="inlineStr"/>
@@ -15582,8 +15746,16 @@
           <t>IpiNivo_Complete_PBMC_CS</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
@@ -15623,8 +15795,16 @@
           <t>IpiNivo_Complete_PBMC_SC</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
@@ -15664,8 +15844,16 @@
           <t>IpiNivo_Complete_kidney_CS</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
@@ -15705,8 +15893,16 @@
           <t>IpiNivo_Complete_kidney_SC</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
@@ -15746,8 +15942,16 @@
           <t>IpiNivo_Complete_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
@@ -15787,8 +15991,16 @@
           <t>IpiNivo_Complete_tumor_Far_SC</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
@@ -15828,8 +16040,16 @@
           <t>IpiNivo_Complete_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
@@ -15869,8 +16089,16 @@
           <t>IpiNivo_Complete_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
@@ -15910,8 +16138,16 @@
           <t>IpiNivo_Mixed_PBMC_CS</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
@@ -15951,8 +16187,16 @@
           <t>IpiNivo_Mixed_kidney_CS</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
@@ -15992,8 +16236,16 @@
           <t>IpiNivo_Mixed_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
@@ -16033,8 +16285,16 @@
           <t>IpiNivo_Mixed_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
@@ -16074,8 +16334,16 @@
           <t>IpiNivo_Mixed_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
@@ -16115,8 +16383,16 @@
           <t>IpiNivo_Resistant_PBMC_CS</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
@@ -16156,8 +16432,16 @@
           <t>IpiNivo_Resistant_kidney_CS</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
@@ -16197,8 +16481,16 @@
           <t>IpiNivo_Resistant_lymph_node_CS</t>
         </is>
       </c>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
@@ -16238,8 +16530,16 @@
           <t>IpiNivo_Resistant_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
@@ -16279,8 +16579,16 @@
           <t>IpiNivo_Resistant_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
@@ -16320,8 +16628,16 @@
           <t>IpiNivo_Resistant_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
@@ -16361,8 +16677,16 @@
           <t>NivoExposed_PBMC_CS</t>
         </is>
       </c>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
@@ -16402,8 +16726,16 @@
           <t>NivoExposed_kidney_CS</t>
         </is>
       </c>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
@@ -16443,8 +16775,16 @@
           <t>NivoExposed_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
@@ -16484,8 +16824,16 @@
           <t>NivoExposed_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
@@ -16525,8 +16873,16 @@
           <t>NivoExposed_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
@@ -16566,8 +16922,16 @@
           <t>UT1_kidney_CS</t>
         </is>
       </c>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
@@ -16607,8 +16971,16 @@
           <t>UT1_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
@@ -16648,8 +17020,16 @@
           <t>UT1_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
@@ -16689,8 +17069,16 @@
           <t>UT1_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
@@ -16730,8 +17118,16 @@
           <t>UT2_kidney_CS</t>
         </is>
       </c>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
@@ -16771,8 +17167,16 @@
           <t>UT2_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
@@ -16812,8 +17216,16 @@
           <t>UT2_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
@@ -16853,8 +17265,16 @@
           <t>UT2_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>library_preparation_protocol_1</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>sequencing_protocol_1</t>
+        </is>
+      </c>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
@@ -17540,11 +17960,7 @@
       <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>enrichment_protocol_1</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
@@ -17564,7 +17980,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>enrichment_protocol_2</t>
+          <t>enrichment_protocol_1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>

</xml_diff>